<commit_message>
B matrix gelukt, even proberen stap 1 apart te maken en dan loop van 2 tot 40
</commit_message>
<xml_diff>
--- a/PCAstatic/predicted_factors_lange_loop.xlsx
+++ b/PCAstatic/predicted_factors_lange_loop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thesis\04. Models\PCAstatic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1D907B-3739-4724-B608-24DF1AB86671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F14AE32-BB2E-4059-80D1-9A40E3F5053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51720" yWindow="-5475" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,121 +187,121 @@
                   <c:v>-1.5429051120952959</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.409825712524021</c:v>
+                  <c:v>-1.4054121915361539</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.28502275575417</c:v>
+                  <c:v>-1.293949753378278</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.1688465101693779</c:v>
+                  <c:v>-1.2044542382113801</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.061593974920823</c:v>
+                  <c:v>-1.133425809274847</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.9635013501373817</c:v>
+                  <c:v>-1.0779292878045279</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.87474373827924123</c:v>
+                  <c:v>-1.035499008251173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.79543595354108143</c:v>
+                  <c:v>-1.0040548908145881</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.72563383808744653</c:v>
+                  <c:v>-0.98183471572602543</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.66533598682880268</c:v>
+                  <c:v>-0.96733983345828523</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.61448582917318617</c:v>
+                  <c:v>-0.95929153638365805</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.5729740221981322</c:v>
+                  <c:v>-0.95659584216679316</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.54064111254723568</c:v>
+                  <c:v>-0.95831490957727372</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.5172804272445759</c:v>
+                  <c:v>-0.96364368854812466</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.50264115662357001</c:v>
+                  <c:v>-0.97189070956003465</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.49643159553007982</c:v>
+                  <c:v>-0.98246215680445625</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.49832251174724451</c:v>
+                  <c:v>-0.99484855751386669</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.50795061310859568</c:v>
+                  <c:v>-1.008613566790127</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.52492208696320342</c:v>
+                  <c:v>-1.022323636179858</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.5488161875146248</c:v>
+                  <c:v>-1.036734195472987</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.57918884808561355</c:v>
+                  <c:v>-1.051569821927345</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.61557629659778945</c:v>
+                  <c:v>-1.066600903244219</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.6574986535509596</c:v>
+                  <c:v>-1.08163715913555</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.70446349260181695</c:v>
+                  <c:v>-1.0965223155824619</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.75596934454282294</c:v>
+                  <c:v>-1.1111294864908019</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.811509126134076</c:v>
+                  <c:v>-1.125357137063481</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.8705734759048418</c:v>
+                  <c:v>-1.139125546122651</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.93265397976883291</c:v>
+                  <c:v>-1.152373701089608</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.99724627012949574</c:v>
+                  <c:v>-1.165056570756656</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-1.063852983117018</c:v>
+                  <c:v>-1.1771427098071141</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-1.1319865597132519</c:v>
+                  <c:v>-1.188612155984714</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-1.201171877787425</c:v>
+                  <c:v>-1.1994545863413399</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-1.270948703476106</c:v>
+                  <c:v>-1.2096677034417589</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-1.34087395187767</c:v>
+                  <c:v>-1.219255826032293</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-1.4105237486693849</c:v>
+                  <c:v>-1.228228661679404</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-1.479495285964127</c:v>
+                  <c:v>-1.2366002413991219</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-1.5474084674710129</c:v>
+                  <c:v>-1.2443879984377919</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-1.6139073397771899</c:v>
+                  <c:v>-1.251611975209971</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-1.678661308295488</c:v>
+                  <c:v>-1.2582941440117339</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-1.741366138096877</c:v>
+                  <c:v>-1.264457828552529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -309,7 +309,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1B5D-47D9-B2CB-2542D0C4DCE8}"/>
+              <c16:uniqueId val="{00000000-E5EF-4335-ABEE-E75DA04047EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -338,121 +338,121 @@
                   <c:v>-0.51878223589789341</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.68269094148024556</c:v>
+                  <c:v>-0.63557723223811224</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.83368625431279919</c:v>
+                  <c:v>-0.72113600732856564</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.97141308765490642</c:v>
+                  <c:v>-0.78107235678347686</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.095643876226621</c:v>
+                  <c:v>-0.81989895798035251</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.206260699804647</c:v>
+                  <c:v>-0.8414527725972486</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.3032514252040279</c:v>
+                  <c:v>-0.84900475963256183</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.3867053825214231</c:v>
+                  <c:v>-0.84533717945727538</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.456807539267849</c:v>
+                  <c:v>-0.8328104294569868</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.513831405720353</c:v>
+                  <c:v>-0.81342120656094929</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.558131036405322</c:v>
+                  <c:v>-0.78885277716220137</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.590132492438489</c:v>
+                  <c:v>-0.76051827703110342</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.6103250955294219</c:v>
+                  <c:v>-0.72959799475618725</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.619252753215696</c:v>
+                  <c:v>-0.69707152298839414</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.6175055750888681</c:v>
+                  <c:v>-0.66374555207583108</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.605711938416531</c:v>
+                  <c:v>-0.63027796397432201</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-1.584531103963263</c:v>
+                  <c:v>-0.59719877599441207</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-1.554646432496223</c:v>
+                  <c:v>-0.56492838983361904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-1.5167592113140549</c:v>
+                  <c:v>-0.53200925404654298</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.4715830687222831</c:v>
+                  <c:v>-0.50076230417338918</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.419838932305459</c:v>
+                  <c:v>-0.47133994222676862</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-1.3622504731335601</c:v>
+                  <c:v>-0.44383717195189892</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-1.2995399714073681</c:v>
+                  <c:v>-0.41830103106227479</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-1.23242453813118</c:v>
+                  <c:v>-0.3947394937621741</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-1.1616126308921091</c:v>
+                  <c:v>-0.37312918007788631</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-1.0878008085442921</c:v>
+                  <c:v>-0.35342196059966058</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-1.011670678520793</c:v>
+                  <c:v>-0.33555058841501723</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.93388600075920392</c:v>
+                  <c:v>-0.31943347824708851</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.85508992310025655</c:v>
+                  <c:v>-0.30497873890637972</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.77590233389016239</c:v>
+                  <c:v>-0.29208755293261401</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.69691732787024363</c:v>
+                  <c:v>-0.28065698667738997</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.61870079083771479</c:v>
+                  <c:v>-0.2705823047701082</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.54178811664795223</c:v>
+                  <c:v>-0.26175885468378629</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.46668207661512889</c:v>
+                  <c:v>-0.25408357979659729</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.39385086604511321</c:v>
+                  <c:v>-0.2474562127943177</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.32372635537811578</c:v>
+                  <c:v>-0.2417801953755126</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.25670257419523351</c:v>
+                  <c:v>-0.23696336492459111</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.1931344552143559</c:v>
+                  <c:v>-0.23291844404380971</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.1333368625216042</c:v>
+                  <c:v>-0.2295633645313328</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-7.7583923894503221E-2</c:v>
+                  <c:v>-0.22682145351460331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -460,7 +460,460 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1B5D-47D9-B2CB-2542D0C4DCE8}"/>
+              <c16:uniqueId val="{00000001-E5EF-4335-ABEE-E75DA04047EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>-0.97155118715070066</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.7907107896782084</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.63328571058107541</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.50028935836751975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.38844180616478208</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.29463723091072569</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.216220587448928</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.1509362197989364</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9.6863296629186191E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.2361263329525183E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.602503483633224E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.33518235395193E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6807445798906872E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5236768764951642E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.9412372958285576E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.0001854433279729E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.7582369540076796E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.2652872442564066E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.5024906337447049E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5695283590095354E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.50185541644223E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.3284035052691602E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.0735562009697457E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.7578497200119246E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.3984969260855788E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.0098357588348768E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.6037195369047558E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.1898580124973618E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.7761160006028318E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.3687751766497297E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.9727637012764408E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.591857595858854E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.2288572094118517E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.8857416511973027E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.5638036866011568E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.2637672856685287E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.9858897581381558E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7300501938026427E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.4958257434271479E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.2825571164716641E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E5EF-4335-ABEE-E75DA04047EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>-0.71385227680948615</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.61475144891046396</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.52433346079146859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.44112611489921449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.36536724264756132</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.29713799424681347</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.2363027949714957</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.18257090692320771</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.1355492967518418</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.4781785127961704E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.9777775699161519E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-3.0033317575077281E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-5.0464486766967302E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5671785699816799E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.2589612935976099E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.6149338626376102E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.6764084956508067E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4816002320425808E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.0114220319200518E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.3509839369393828E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.5309891991658287E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.5791714408832644E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.5199727654921514E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.3747591832185086E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.1620807300276743E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.8979305700444596E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.5959954906579979E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.2678945176137743E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.9234036544095293E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.5706655628335357E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.2163836069902381E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.8660001391482938E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.5238592454315177E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.1933544178390778E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.8770617959605853E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5768597425364652E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.2940355939605592E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.0293804696640812E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.783273040813198E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.5557531550884E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E5EF-4335-ABEE-E75DA04047EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.82313366247467901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63300705902108534</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.48528590594881899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.36956891065308112</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2788732848954904</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20784684360584699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15231228210553241</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1089951328195647</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5322013595805551E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9266127149193657E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9228056743120921E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.394341138795854E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4110356412266548E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-6.1629536789138241E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.240890191483237E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.6827870789529711E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.9818522549312729E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-2.1698260636456371E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-2.2517976555055701E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-2.2713188531636751E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-2.244179522555555E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-2.1830742700994301E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-2.0979637386697381E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-1.9966206952880049E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-1.8850815712756409E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.7680046737528519E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.648953823103794E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.53062342273317E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-1.415017512275E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-1.3035925764883639E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.1973717244106801E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-1.097036183032407E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.0029987561472289E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-9.1546289621595167E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-8.3447025875044295E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-7.5993900374168579E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-6.9169463757086328E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-6.2949482123982707E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-5.7304928317529948E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-5.2203574922051422E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E5EF-4335-ABEE-E75DA04047EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -473,11 +926,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="102696000"/>
-        <c:axId val="102706080"/>
+        <c:axId val="548502367"/>
+        <c:axId val="548503327"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102696000"/>
+        <c:axId val="548502367"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,7 +972,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102706080"/>
+        <c:crossAx val="548503327"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -527,7 +980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102706080"/>
+        <c:axId val="548503327"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -578,7 +1031,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102696000"/>
+        <c:crossAx val="548502367"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1225,23 +1678,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>536575</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>231775</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62E8CABD-34C2-98BD-706F-373279681465}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD5CEC38-5AC9-323B-D4D7-AC509C330BB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1549,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1591,665 +2044,665 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>-1.409825712524021</v>
+        <v>-1.4054121915361539</v>
       </c>
       <c r="B3">
-        <v>-0.68269094148024556</v>
+        <v>-0.63557723223811224</v>
       </c>
       <c r="C3">
-        <v>-0.89916366020775518</v>
+        <v>-0.7907107896782084</v>
       </c>
       <c r="D3">
-        <v>-0.68255757951990059</v>
+        <v>-0.61475144891046396</v>
       </c>
       <c r="E3">
-        <v>0.75420359606052512</v>
+        <v>0.63300705902108534</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>-1.28502275575417</v>
+        <v>-1.293949753378278</v>
       </c>
       <c r="B4">
-        <v>-0.83368625431279919</v>
+        <v>-0.72113600732856564</v>
       </c>
       <c r="C4">
-        <v>-0.82495681412353106</v>
+        <v>-0.63328571058107541</v>
       </c>
       <c r="D4">
-        <v>-0.64554559505758602</v>
+        <v>-0.52433346079146859</v>
       </c>
       <c r="E4">
-        <v>0.68804390722567665</v>
+        <v>0.48528590594881899</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>-1.1688465101693779</v>
+        <v>-1.2044542382113801</v>
       </c>
       <c r="B5">
-        <v>-0.97141308765490642</v>
+        <v>-0.78107235678347686</v>
       </c>
       <c r="C5">
-        <v>-0.74914520077710034</v>
+        <v>-0.50028935836751975</v>
       </c>
       <c r="D5">
-        <v>-0.60357119533832571</v>
+        <v>-0.44112611489921449</v>
       </c>
       <c r="E5">
-        <v>0.62474096460212081</v>
+        <v>0.36956891065308112</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>-1.061593974920823</v>
+        <v>-1.133425809274847</v>
       </c>
       <c r="B6">
-        <v>-1.095643876226621</v>
+        <v>-0.81989895798035251</v>
       </c>
       <c r="C6">
-        <v>-0.67222950600031417</v>
+        <v>-0.38844180616478208</v>
       </c>
       <c r="D6">
-        <v>-0.55728433335192828</v>
+        <v>-0.36536724264756132</v>
       </c>
       <c r="E6">
-        <v>0.56431412865246522</v>
+        <v>0.2788732848954904</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>-0.9635013501373817</v>
+        <v>-1.0779292878045279</v>
       </c>
       <c r="B7">
-        <v>-1.206260699804647</v>
+        <v>-0.8414527725972486</v>
       </c>
       <c r="C7">
-        <v>-0.59474812177921166</v>
+        <v>-0.29463723091072569</v>
       </c>
       <c r="D7">
-        <v>-0.50731969098290097</v>
+        <v>-0.29713799424681347</v>
       </c>
       <c r="E7">
-        <v>0.50677452397747635</v>
+        <v>0.20784684360584699</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>-0.87474373827924123</v>
+        <v>-1.035499008251173</v>
       </c>
       <c r="B8">
-        <v>-1.3032514252040279</v>
+        <v>-0.84900475963256183</v>
       </c>
       <c r="C8">
-        <v>-0.51724283425305773</v>
+        <v>-0.216220587448928</v>
       </c>
       <c r="D8">
-        <v>-0.45430026110310429</v>
+        <v>-0.2363027949714957</v>
       </c>
       <c r="E8">
-        <v>0.45213017312155929</v>
+        <v>0.15231228210553241</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>-0.79543595354108143</v>
+        <v>-1.0040548908145881</v>
       </c>
       <c r="B9">
-        <v>-1.3867053825214231</v>
+        <v>-0.84533717945727538</v>
       </c>
       <c r="C9">
-        <v>-0.44024479101275482</v>
+        <v>-0.1509362197989364</v>
       </c>
       <c r="D9">
-        <v>-0.39883351218972812</v>
+        <v>-0.18257090692320771</v>
       </c>
       <c r="E9">
-        <v>0.40038617848539459</v>
+        <v>0.1089951328195647</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>-0.72563383808744653</v>
+        <v>-0.98183471572602543</v>
       </c>
       <c r="B10">
-        <v>-1.456807539267849</v>
+        <v>-0.8328104294569868</v>
       </c>
       <c r="C10">
-        <v>-0.36426364132403738</v>
+        <v>-9.6863296629186191E-2</v>
       </c>
       <c r="D10">
-        <v>-0.34150733174040931</v>
+        <v>-0.1355492967518418</v>
       </c>
       <c r="E10">
-        <v>0.35154433808031532</v>
+        <v>7.5322013595805551E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>-0.66533598682880268</v>
+        <v>-0.96733983345828523</v>
       </c>
       <c r="B11">
-        <v>-1.513831405720353</v>
+        <v>-0.81342120656094929</v>
       </c>
       <c r="C11">
-        <v>-0.28977860958632018</v>
+        <v>-5.2361263329525183E-2</v>
       </c>
       <c r="D11">
-        <v>-0.28288643514444739</v>
+        <v>-9.4781785127961704E-2</v>
       </c>
       <c r="E11">
-        <v>0.30560259866312528</v>
+        <v>4.9266127149193657E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>-0.61448582917318617</v>
+        <v>-0.95929153638365805</v>
       </c>
       <c r="B12">
-        <v>-1.558131036405322</v>
+        <v>-0.78885277716220137</v>
       </c>
       <c r="C12">
-        <v>-0.21723155288215221</v>
+        <v>-1.602503483633224E-2</v>
       </c>
       <c r="D12">
-        <v>-0.2235093194154118</v>
+        <v>-5.9777775699161519E-2</v>
       </c>
       <c r="E12">
-        <v>0.26255440624813398</v>
+        <v>2.9228056743120921E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>-0.5729740221981322</v>
+        <v>-0.95659584216679316</v>
       </c>
       <c r="B13">
-        <v>-1.590132492438489</v>
+        <v>-0.76051827703110342</v>
       </c>
       <c r="C13">
-        <v>-0.14702203330536531</v>
+        <v>1.33518235395193E-2</v>
       </c>
       <c r="D13">
-        <v>-0.16388576982112399</v>
+        <v>-3.0033317575077281E-2</v>
       </c>
       <c r="E13">
-        <v>0.22238799327311259</v>
+        <v>1.394341138795854E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>-0.54064111254723568</v>
+        <v>-0.95831490957727372</v>
       </c>
       <c r="B14">
-        <v>-1.6103250955294219</v>
+        <v>-0.72959799475618725</v>
       </c>
       <c r="C14">
-        <v>-7.9504317808513553E-2</v>
+        <v>3.6807445798906872E-2</v>
       </c>
       <c r="D14">
-        <v>-0.1044949054171533</v>
+        <v>-5.0464486766967302E-3</v>
       </c>
       <c r="E14">
-        <v>0.18508564491063209</v>
+        <v>2.4110356412266548E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>-0.5172804272445759</v>
+        <v>-0.96364368854812466</v>
       </c>
       <c r="B15">
-        <v>-1.619252753215696</v>
+        <v>-0.69707152298839414</v>
       </c>
       <c r="C15">
-        <v>-1.498611905696361E-2</v>
+        <v>5.5236768764951642E-2</v>
       </c>
       <c r="D15">
-        <v>-4.5783733703647897E-2</v>
+        <v>1.5671785699816799E-2</v>
       </c>
       <c r="E15">
-        <v>0.1506229881567856</v>
+        <v>-6.1629536789138241E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>-0.50264115662357001</v>
+        <v>-0.97189070956003465</v>
       </c>
       <c r="B16">
-        <v>-1.6175055750888681</v>
+        <v>-0.66374555207583108</v>
       </c>
       <c r="C16">
-        <v>4.6271177049593298E-2</v>
+        <v>6.9412372958285576E-2</v>
       </c>
       <c r="D16">
-        <v>1.1833827956687909E-2</v>
+        <v>3.2589612935976099E-2</v>
       </c>
       <c r="E16">
-        <v>0.118968345027194</v>
+        <v>-1.240890191483237E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>-0.49643159553007982</v>
+        <v>-0.98246215680445625</v>
       </c>
       <c r="B17">
-        <v>-1.605711938416531</v>
+        <v>-0.63027796397432201</v>
       </c>
       <c r="C17">
-        <v>0.10405108818002611</v>
+        <v>8.0001854433279729E-2</v>
       </c>
       <c r="D17">
-        <v>6.7977515612119996E-2</v>
+        <v>4.6149338626376102E-2</v>
       </c>
       <c r="E17">
-        <v>9.0082186216795687E-2</v>
+        <v>-1.6827870789529711E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>-0.49832251174724451</v>
+        <v>-0.99484855751386669</v>
       </c>
       <c r="B18">
-        <v>-1.584531103963263</v>
+        <v>-0.59719877599441207</v>
       </c>
       <c r="C18">
-        <v>0.1581797170633687</v>
+        <v>8.7582369540076796E-2</v>
       </c>
       <c r="D18">
-        <v>0.12230092348613431</v>
+        <v>5.6764084956508067E-2</v>
       </c>
       <c r="E18">
-        <v>6.3916714791791382E-2</v>
+        <v>-1.9818522549312729E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>-0.50795061310859568</v>
+        <v>-1.008613566790127</v>
       </c>
       <c r="B19">
-        <v>-1.554646432496223</v>
+        <v>-0.56492838983361904</v>
       </c>
       <c r="C19">
-        <v>0.20852282568196059</v>
+        <v>9.2652872442564066E-2</v>
       </c>
       <c r="D19">
-        <v>0.17449140869986299</v>
+        <v>6.4816002320425808E-2</v>
       </c>
       <c r="E19">
-        <v>4.0415601629499698E-2</v>
+        <v>-2.1698260636456371E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>-0.52492208696320342</v>
+        <v>-1.022323636179858</v>
       </c>
       <c r="B20">
-        <v>-1.5167592113140549</v>
+        <v>-0.53200925404654298</v>
       </c>
       <c r="C20">
-        <v>0.25498256216856668</v>
+        <v>9.5024906337447049E-2</v>
       </c>
       <c r="D20">
-        <v>0.22426975276460959</v>
+        <v>7.0114220319200518E-2</v>
       </c>
       <c r="E20">
-        <v>1.951388603735164E-2</v>
+        <v>-2.2517976555055701E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>-0.5488161875146248</v>
+        <v>-1.036734195472987</v>
       </c>
       <c r="B21">
-        <v>-1.4715830687222831</v>
+        <v>-0.50076230417338918</v>
       </c>
       <c r="C21">
-        <v>0.29749406251073862</v>
+        <v>9.5695283590095354E-2</v>
       </c>
       <c r="D21">
-        <v>0.271389632246476</v>
+        <v>7.3509839369393828E-2</v>
       </c>
       <c r="E21">
-        <v>1.138046787650848E-3</v>
+        <v>-2.2713188531636751E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>-0.57918884808561355</v>
+        <v>-1.051569821927345</v>
       </c>
       <c r="B22">
-        <v>-1.419838932305459</v>
+        <v>-0.47133994222676862</v>
       </c>
       <c r="C22">
-        <v>0.33602210635266738</v>
+        <v>9.50185541644223E-2</v>
       </c>
       <c r="D22">
-        <v>0.31563694453875352</v>
+        <v>7.5309891991658287E-2</v>
       </c>
       <c r="E22">
-        <v>-1.479375887821425E-2</v>
+        <v>-2.244179522555555E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>-0.61557629659778945</v>
+        <v>-1.066600903244219</v>
       </c>
       <c r="B23">
-        <v>-1.3622504731335601</v>
+        <v>-0.44383717195189892</v>
       </c>
       <c r="C23">
-        <v>0.37055796240557881</v>
+        <v>9.3284035052691602E-2</v>
       </c>
       <c r="D23">
-        <v>0.35682902690025342</v>
+        <v>7.5791714408832644E-2</v>
       </c>
       <c r="E23">
-        <v>-2.8371297563300129E-2</v>
+        <v>-2.1830742700994301E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>-0.6574986535509596</v>
+        <v>-1.08163715913555</v>
       </c>
       <c r="B24">
-        <v>-1.2995399714073681</v>
+        <v>-0.41830103106227479</v>
       </c>
       <c r="C24">
-        <v>0.40111651712710689</v>
+        <v>9.0735562009697457E-2</v>
       </c>
       <c r="D24">
-        <v>0.39481379855068433</v>
+        <v>7.5199727654921514E-2</v>
       </c>
       <c r="E24">
-        <v>-3.96917183869007E-2</v>
+        <v>-2.0979637386697381E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>-0.70446349260181695</v>
+        <v>-1.0965223155824619</v>
       </c>
       <c r="B25">
-        <v>-1.23242453813118</v>
+        <v>-0.3947394937621741</v>
       </c>
       <c r="C25">
-        <v>0.42773374234722861</v>
+        <v>8.7578497200119246E-2</v>
       </c>
       <c r="D25">
-        <v>0.42946884730169133</v>
+        <v>7.3747591832185086E-2</v>
       </c>
       <c r="E25">
-        <v>-4.8858887555573577E-2</v>
+        <v>-1.9966206952880049E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>-0.75596934454282294</v>
+        <v>-1.1111294864908019</v>
       </c>
       <c r="B26">
-        <v>-1.1616126308921091</v>
+        <v>-0.37312918007788631</v>
       </c>
       <c r="C26">
-        <v>0.4504645245569075</v>
+        <v>8.3984969260855788E-2</v>
       </c>
       <c r="D26">
-        <v>0.46070047447450813</v>
+        <v>7.1620807300276743E-2</v>
       </c>
       <c r="E26">
-        <v>-5.5982621534048468E-2</v>
+        <v>-1.8850815712756409E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>-0.811509126134076</v>
+        <v>-1.125357137063481</v>
       </c>
       <c r="B27">
-        <v>-1.0878008085442921</v>
+        <v>-0.35342196059966058</v>
       </c>
       <c r="C27">
-        <v>0.46938085118815193</v>
+        <v>8.0098357588348768E-2</v>
       </c>
       <c r="D27">
-        <v>0.48844270511046539</v>
+        <v>6.8979305700444596E-2</v>
       </c>
       <c r="E27">
-        <v>-6.1177843321483003E-2</v>
+        <v>-1.7680046737528519E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>-0.8705734759048418</v>
+        <v>-1.139125546122651</v>
       </c>
       <c r="B28">
-        <v>-1.011670678520793</v>
+        <v>-0.33555058841501723</v>
       </c>
       <c r="C28">
-        <v>0.48457032752512191</v>
+        <v>7.6037195369047558E-2</v>
       </c>
       <c r="D28">
-        <v>0.51265626498096495</v>
+        <v>6.5959954906579979E-2</v>
       </c>
       <c r="E28">
-        <v>-6.4563686843947143E-2</v>
+        <v>-1.648953823103794E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>-0.93265397976883291</v>
+        <v>-1.152373701089608</v>
       </c>
       <c r="B29">
-        <v>-0.93388600075920392</v>
+        <v>-0.31943347824708851</v>
       </c>
       <c r="C29">
-        <v>0.49613498173487097</v>
+        <v>7.1898580124973618E-2</v>
       </c>
       <c r="D29">
-        <v>0.53332752178349918</v>
+        <v>6.2678945176137743E-2</v>
       </c>
       <c r="E29">
-        <v>-6.6262573797657334E-2</v>
+        <v>-1.53062342273317E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>-0.99724627012949574</v>
+        <v>-1.165056570756656</v>
       </c>
       <c r="B30">
-        <v>-0.85508992310025655</v>
+        <v>-0.30497873890637972</v>
       </c>
       <c r="C30">
-        <v>0.50419030455492775</v>
+        <v>6.7761160006028318E-2</v>
       </c>
       <c r="D30">
-        <v>0.55046738519339744</v>
+        <v>5.9234036544095293E-2</v>
       </c>
       <c r="E30">
-        <v>-6.6399285588710985E-2</v>
+        <v>-1.415017512275E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>-1.063852983117018</v>
+        <v>-1.1771427098071141</v>
       </c>
       <c r="B31">
-        <v>-0.77590233389016239</v>
+        <v>-0.29208755293261401</v>
       </c>
       <c r="C31">
-        <v>0.50886446397925578</v>
+        <v>6.3687751766497297E-2</v>
       </c>
       <c r="D31">
-        <v>0.56411015905983508</v>
+        <v>5.5706655628335357E-2</v>
       </c>
       <c r="E31">
-        <v>-6.5100050522377675E-2</v>
+        <v>-1.3035925764883639E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>-1.1319865597132519</v>
+        <v>-1.188612155984714</v>
       </c>
       <c r="B32">
-        <v>-0.69691732787024363</v>
+        <v>-0.28065698667738997</v>
       </c>
       <c r="C32">
-        <v>0.51029763333841172</v>
+        <v>5.9727637012764408E-2</v>
       </c>
       <c r="D32">
-        <v>0.57431233885496513</v>
+        <v>5.2163836069902381E-2</v>
       </c>
       <c r="E32">
-        <v>-6.249166332957734E-2</v>
+        <v>-1.1973717244106801E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>-1.201171877787425</v>
+        <v>-1.1994545863413399</v>
       </c>
       <c r="B33">
-        <v>-0.61870079083771479</v>
+        <v>-0.2705823047701082</v>
       </c>
       <c r="C33">
-        <v>0.50864137292829115</v>
+        <v>5.591857595858854E-2</v>
       </c>
       <c r="D33">
-        <v>0.58115134832524651</v>
+        <v>4.8660001391482938E-2</v>
       </c>
       <c r="E33">
-        <v>-5.87006507188262E-2</v>
+        <v>-1.097036183032407E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>-1.270948703476106</v>
+        <v>-1.2096677034417589</v>
       </c>
       <c r="B34">
-        <v>-0.54178811664795223</v>
+        <v>-0.26175885468378629</v>
       </c>
       <c r="C34">
-        <v>0.50405801022843988</v>
+        <v>5.2288572094118517E-2</v>
       </c>
       <c r="D34">
-        <v>0.58472421094678018</v>
+        <v>4.5238592454315177E-2</v>
       </c>
       <c r="E34">
-        <v>-5.3852493137537177E-2</v>
+        <v>-1.0029987561472289E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>-1.34087395187767</v>
+        <v>-1.219255826032293</v>
       </c>
       <c r="B35">
-        <v>-0.46668207661512889</v>
+        <v>-0.25408357979659729</v>
       </c>
       <c r="C35">
-        <v>0.49671997116131988</v>
+        <v>4.8857416511973027E-2</v>
       </c>
       <c r="D35">
-        <v>0.58514615403290393</v>
+        <v>4.1933544178390778E-2</v>
       </c>
       <c r="E35">
-        <v>-4.807090952366732E-2</v>
+        <v>-9.1546289621595167E-3</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>-1.4105237486693849</v>
+        <v>-1.228228661679404</v>
       </c>
       <c r="B36">
-        <v>-0.39385086604511321</v>
+        <v>-0.2474562127943177</v>
       </c>
       <c r="C36">
-        <v>0.48680902414961141</v>
+        <v>4.5638036866011568E-2</v>
       </c>
       <c r="D36">
-        <v>0.58254914596654372</v>
+        <v>3.8770617959605853E-2</v>
       </c>
       <c r="E36">
-        <v>-4.1477208699083591E-2</v>
+        <v>-8.3447025875044295E-3</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>-1.479495285964127</v>
+        <v>-1.2366002413991219</v>
       </c>
       <c r="B37">
-        <v>-0.32372635537811578</v>
+        <v>-0.2417801953755126</v>
       </c>
       <c r="C37">
-        <v>0.47451540928403968</v>
+        <v>4.2637672856685287E-2</v>
       </c>
       <c r="D37">
-        <v>0.57708036982752997</v>
+        <v>3.5768597425364652E-2</v>
       </c>
       <c r="E37">
-        <v>-3.418970833049962E-2</v>
+        <v>-7.5993900374168579E-3</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>-1.5474084674710129</v>
+        <v>-1.2443879984377919</v>
       </c>
       <c r="B38">
-        <v>-0.25670257419523351</v>
+        <v>-0.23696336492459111</v>
       </c>
       <c r="C38">
-        <v>0.46003683607012308</v>
+        <v>3.9858897581381558E-2</v>
       </c>
       <c r="D38">
-        <v>0.56890063947170233</v>
+        <v>3.2940355939605592E-2</v>
       </c>
       <c r="E38">
-        <v>-2.632322014828993E-2</v>
+        <v>-6.9169463757086328E-3</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>-1.6139073397771899</v>
+        <v>-1.251611975209971</v>
       </c>
       <c r="B39">
-        <v>-0.1931344552143559</v>
+        <v>-0.23291844404380971</v>
       </c>
       <c r="C39">
-        <v>0.44357734434696439</v>
+        <v>3.7300501938026427E-2</v>
       </c>
       <c r="D39">
-        <v>0.55818276673344802</v>
+        <v>3.0293804696640812E-2</v>
       </c>
       <c r="E39">
-        <v>-1.79885984102089E-2</v>
+        <v>-6.2949482123982707E-3</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>-1.678661308295488</v>
+        <v>-1.2582941440117339</v>
       </c>
       <c r="B40">
-        <v>-0.1333368625216042</v>
+        <v>-0.2295633645313328</v>
       </c>
       <c r="C40">
-        <v>0.42534603347496031</v>
+        <v>3.4958257434271479E-2</v>
       </c>
       <c r="D40">
-        <v>0.54510989073382143</v>
+        <v>2.783273040813198E-2</v>
       </c>
       <c r="E40">
-        <v>-9.2923474278298786E-3</v>
+        <v>-5.7304928317529948E-3</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>-1.741366138096877</v>
+        <v>-1.264457828552529</v>
       </c>
       <c r="B41">
-        <v>-7.7583923894503221E-2</v>
+        <v>-0.22682145351460331</v>
       </c>
       <c r="C41">
-        <v>0.40555567425321443</v>
+        <v>3.2825571164716641E-2</v>
       </c>
       <c r="D41">
-        <v>0.52987378217959213</v>
+        <v>2.5557531550884E-2</v>
       </c>
       <c r="E41">
-        <v>-3.3628330677462111E-4</v>
+        <v>-5.2203574922051422E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bezig met test train split, was statisch, wordt nu cross-validated om de B matrix te optimaliseren
</commit_message>
<xml_diff>
--- a/PCAstatic/predicted_factors_lange_loop.xlsx
+++ b/PCAstatic/predicted_factors_lange_loop.xlsx
@@ -462,682 +462,682 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1.542905112095296</v>
+        <v>-4.377829468602984</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.5187822358978934</v>
+        <v>-3.038932295093685</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.9715511871507007</v>
+        <v>0.2056286196336669</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.7138522768094862</v>
+        <v>-0.1561269739048682</v>
       </c>
       <c r="E2" t="n">
-        <v>0.823133662474679</v>
+        <v>0.3138575077444884</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-1.405412191536154</v>
+        <v>-4.135240465056005</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.6355772322381122</v>
+        <v>-2.925761869611146</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.7907107896782084</v>
+        <v>0.1526961756983606</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.614751448910464</v>
+        <v>-0.007081435956113867</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6330070590210853</v>
+        <v>0.1996924965362855</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-1.294224018327199</v>
+        <v>-3.91779440813451</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.7215351984235536</v>
+        <v>-2.786980976820223</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.6329346711635021</v>
+        <v>0.2116711397399643</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.5246384838954793</v>
+        <v>0.06285134145811457</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4842658382665657</v>
+        <v>0.1409986714813057</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-1.20523260650188</v>
+        <v>-3.727207631739984</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.7820258320913909</v>
+        <v>-2.63896785544131</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.4992725093220444</v>
+        <v>0.266773802289977</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.4415632484604988</v>
+        <v>0.1151279292582288</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3672961107578325</v>
+        <v>0.09726210584603523</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-1.134908612556534</v>
+        <v>-3.560370163304749</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.8213394538761309</v>
+        <v>-2.486596470533827</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.3865544462597956</v>
+        <v>0.3083680167545987</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.3656083637111721</v>
+        <v>0.156400625316125</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2754586733569139</v>
+        <v>0.06290010432766577</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-1.080293837538196</v>
+        <v>-3.4140320213363</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.8431533209152763</v>
+        <v>-2.333043362829101</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.2917820634978145</v>
+        <v>0.3373751349543979</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.2968637330054407</v>
+        <v>0.1880986218500402</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2035313365040343</v>
+        <v>0.03601604595621438</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-1.038901291561954</v>
+        <v>-3.285267012599882</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.8506462001897463</v>
+        <v>-2.180799115878838</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.2123918020348036</v>
+        <v>0.3556584128154492</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.2352726129329367</v>
+        <v>0.2112694803727222</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1473643750284583</v>
+        <v>0.01526419832980576</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-1.008628911021791</v>
+        <v>-3.171504433694817</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.8465654890000238</v>
+        <v>-2.031820051881835</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.146199600431181</v>
+        <v>0.365023877449405</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.1806427237377109</v>
+        <v>0.2269773108623601</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1036651490791632</v>
+        <v>-0.0004787394824077064</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.9876910704978006</v>
+        <v>-3.070510228545634</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.8332792831198447</v>
+        <v>-1.887602301144848</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0913359305223345</v>
+        <v>0.3671011042269253</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1326740055759211</v>
+        <v>0.2362818665803226</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06982457551723331</v>
+        <v>-0.01216270276063274</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.9745644923680884</v>
+        <v>-2.980358720832418</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.8128201165223894</v>
+        <v>-1.749249412619633</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.04619287388857883</v>
+        <v>0.3633261933465243</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.09098683664380455</v>
+        <v>0.2401960799948154</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0437760434360385</v>
+        <v>-0.02058573907449598</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-0.9679453140702341</v>
+        <v>-2.899401465639657</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.7869231565351705</v>
+        <v>-1.617536338918757</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.009382019179845489</v>
+        <v>0.3549447287318384</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.05514752764789614</v>
+        <v>0.2396572970327526</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02388213351444264</v>
+        <v>-0.02641257492002178</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-0.966714742901027</v>
+        <v>-2.826235676702645</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.7570603054861939</v>
+        <v>-1.492967745081127</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02029922325940038</v>
+        <v>0.3430228639462004</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.02469011803033791</v>
+        <v>0.2355116619108308</v>
       </c>
       <c r="E13" t="n">
-        <v>0.008844546962801172</v>
+        <v>-0.03019228911398673</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-0.9699113168918396</v>
+        <v>-2.75967371208912</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.7244710000081136</v>
+        <v>-1.375829432128243</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04389483852564564</v>
+        <v>0.3284626296547462</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0008657087064025586</v>
+        <v>0.2285081468464749</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.00236707399212796</v>
+        <v>-0.03237490830192973</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-0.9767082608938605</v>
+        <v>-2.698714543450587</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.690190152332067</v>
+        <v>-1.266232600289749</v>
       </c>
       <c r="C15" t="n">
-        <v>0.06231244221377371</v>
+        <v>0.3120191390451815</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0220003924837876</v>
+        <v>0.2192991240412868</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.01057120890976126</v>
+        <v>-0.0333266207866517</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-0.9863947935136861</v>
+        <v>-2.642517725653839</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.6550735009864288</v>
+        <v>-1.16415126757514</v>
       </c>
       <c r="C16" t="n">
-        <v>0.07634165642519268</v>
+        <v>0.2943181525803341</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0391835674711321</v>
+        <v>0.2084450816413542</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.01641855792664058</v>
+        <v>-0.03334340822790796</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-0.9983605214896596</v>
+        <v>-2.59038008719811</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.6198205545195392</v>
+        <v>-1.069453473394109</v>
       </c>
       <c r="C17" t="n">
-        <v>0.08666947300273746</v>
+        <v>0.2758730185441844</v>
       </c>
       <c r="D17" t="n">
-        <v>0.05286598577956164</v>
+        <v>0.1964217272548262</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.02042673496693263</v>
+        <v>-0.03266301278600346</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-1.012082270881919</v>
+        <v>-2.541715157163297</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.584995277433042</v>
+        <v>-0.9819270265325778</v>
       </c>
       <c r="C18" t="n">
-        <v>0.09389324109579922</v>
+        <v>0.2571004096770639</v>
       </c>
       <c r="D18" t="n">
-        <v>0.063473834796429</v>
+        <v>0.1836282471547657</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.02300759332069815</v>
+        <v>-0.03147525679828501</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-1.027112864102592</v>
+        <v>-2.496035212057282</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.5510446574197568</v>
+        <v>-0.9013005735026718</v>
       </c>
       <c r="C19" t="n">
-        <v>0.09853175912170545</v>
+        <v>0.2383345612355345</v>
       </c>
       <c r="D19" t="n">
-        <v>0.07140501445589002</v>
+        <v>0.1703958948165927</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.02448878767118823</v>
+        <v>-0.02993080535515241</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-1.04307147077713</v>
+        <v>-2.452935747855727</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.518315293208729</v>
+        <v>-0.827260716904461</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1010348340667438</v>
+        <v>0.219839908663442</v>
       </c>
       <c r="D20" t="n">
-        <v>0.07702698377200966</v>
+        <v>0.1569963830630042</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.02513082598129538</v>
+        <v>-0.02814850927639157</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-1.059635248676323</v>
+        <v>-2.412082143414136</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.4870681453015716</v>
+        <v>-0.7594658365778045</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1017915842239516</v>
+        <v>0.2018221467515104</v>
       </c>
       <c r="D21" t="n">
-        <v>0.08067583626153521</v>
+        <v>0.1436497688914796</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.02514058684554544</v>
+        <v>-0.02622149068009805</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>-1.076532056288765</v>
+        <v>-2.373198268962183</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.4574915939439813</v>
+        <v>-0.6975571791258875</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1011376973355807</v>
+        <v>0.1844378057736476</v>
       </c>
       <c r="D22" t="n">
-        <v>0.08265631523834774</v>
+        <v>0.1305316681338991</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.02468206067184397</v>
+        <v>-0.02422214067678939</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>-1.093534066991698</v>
+        <v>-2.336056798143359</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.4297129483269714</v>
+        <v>-0.6411676954517767</v>
       </c>
       <c r="C23" t="n">
-        <v>0.09936180883174102</v>
+        <v>0.1678024787530985</v>
       </c>
       <c r="D23" t="n">
-        <v>0.08324252871961223</v>
+        <v>0.1177797353006681</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.02388490451777894</v>
+        <v>-0.02220619385725165</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-1.110452150726531</v>
+        <v>-2.300470997127772</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.4038085479741399</v>
+        <v>-0.589929027279597</v>
       </c>
       <c r="C24" t="n">
-        <v>0.09671112995018559</v>
+        <v>0.1519978492892873</v>
       </c>
       <c r="D24" t="n">
-        <v>0.08267916786703305</v>
+        <v>0.105499406126406</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.02285127019578414</v>
+        <v>-0.02021603166578994</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>-1.127130915940063</v>
+        <v>-2.266287784834241</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.37981259186683</v>
+        <v>-0.5434769747808197</v>
       </c>
       <c r="C25" t="n">
-        <v>0.09339642961449338</v>
+        <v>0.1370776697934964</v>
       </c>
       <c r="D25" t="n">
-        <v>0.08118307161151235</v>
+        <v>0.09376893726324381</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.02166126479249711</v>
+        <v>-0.01828335001598595</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-1.143444324771644</v>
+        <v>-2.233381880963938</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.3577248236544815</v>
+        <v>-0.5014557189097788</v>
       </c>
       <c r="C26" t="n">
-        <v>0.08959645454560364</v>
+        <v>0.1230728316179136</v>
       </c>
       <c r="D26" t="n">
-        <v>0.07894501319259457</v>
+        <v>0.08264379738313567</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.02037732515643726</v>
+        <v>-0.01643130821148723</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-1.159291809841202</v>
+        <v>-2.201650881263391</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.3375171929017848</v>
+        <v>-0.4635210232883112</v>
       </c>
       <c r="C27" t="n">
-        <v>0.08546185736944961</v>
+        <v>0.1099956555985796</v>
       </c>
       <c r="D27" t="n">
-        <v>0.07613161203052872</v>
+        <v>0.07216047257004851</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.01904772783486385</v>
+        <v>-0.01467625813462307</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-1.174594832819441</v>
+        <v>-2.17101112093779</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.3191396032863777</v>
+        <v>-0.4293426003682588</v>
       </c>
       <c r="C28" t="n">
-        <v>0.081118691157476</v>
+        <v>0.09784351672627689</v>
       </c>
       <c r="D28" t="n">
-        <v>0.07288729712368776</v>
+        <v>0.06233975049621875</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.01770940926427705</v>
+        <v>-0.01302913583962656</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-1.189293834175614</v>
+        <v>-2.141394206750376</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.302524849426335</v>
+        <v>-0.3986057938719949</v>
       </c>
       <c r="C29" t="n">
-        <v>0.07667151997114877</v>
+        <v>0.08660190173614611</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0693362666243265</v>
+        <v>0.05318954536745196</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.01639023460160745</v>
+        <v>-0.01149658270986926</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-1.203345530774563</v>
+        <v>-2.112744115783735</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.2875928349191941</v>
+        <v>-0.3710127029166113</v>
       </c>
       <c r="C30" t="n">
-        <v>0.07220618792289138</v>
+        <v>0.07624698436831955</v>
       </c>
       <c r="D30" t="n">
-        <v>0.06558440301589588</v>
+        <v>0.04470732091579457</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.01511082504763315</v>
+        <v>-0.01008185043184822</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-1.216720523821244</v>
+        <v>-2.085014774065904</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.2742541554441061</v>
+        <v>-0.3462828516364005</v>
       </c>
       <c r="C31" t="n">
-        <v>0.06779228355467166</v>
+        <v>0.06674779040933669</v>
       </c>
       <c r="D31" t="n">
-        <v>0.06172111499578666</v>
+        <v>0.03688216305387852</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.01388603106248847</v>
+        <v>-0.008785533194832459</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-1.229401184381704</v>
+        <v>-2.058168041386568</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.2624131225604623</v>
+        <v>-0.3241534905576728</v>
       </c>
       <c r="C32" t="n">
-        <v>0.06348533164700147</v>
+        <v>0.05806801357067486</v>
       </c>
       <c r="D32" t="n">
-        <v>0.05782108630513581</v>
+        <v>0.02969654794681034</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.01272612114276028</v>
+        <v>-0.007606161598544746</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-1.241379787603503</v>
+        <v>-2.032172039833269</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.2519702962078583</v>
+        <v>-0.3043796016399409</v>
       </c>
       <c r="C33" t="n">
-        <v>0.05932874067387407</v>
+        <v>0.05016753379413031</v>
       </c>
       <c r="D33" t="n">
-        <v>0.05394591882162626</v>
+        <v>0.02312784564417318</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.01163774178386683</v>
+        <v>-0.006540685525120827</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-1.252656870006786</v>
+        <v>-2.006999773084602</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.2428245869024327</v>
+        <v>-0.2867336671206656</v>
       </c>
       <c r="C34" t="n">
-        <v>0.05535553084502172</v>
+        <v>0.04300368158159788</v>
       </c>
       <c r="D34" t="n">
-        <v>0.05014566265051051</v>
+        <v>0.01714959427347313</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.01062469309657749</v>
+        <v>-0.00558486746229182</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-1.263239786961714</v>
+        <v>-1.982627991532646</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.2348749822290448</v>
+        <v>-0.2710052525625544</v>
       </c>
       <c r="C35" t="n">
-        <v>0.05158986490131724</v>
+        <v>0.03653228526271295</v>
       </c>
       <c r="D35" t="n">
-        <v>0.04646023005388553</v>
+        <v>0.01173257521948482</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.009688555670904703</v>
+        <v>-0.004733603210405914</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-1.273141449815519</v>
+        <v>-1.959036265084278</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.2280219464217012</v>
+        <v>-0.2570004463902629</v>
       </c>
       <c r="C36" t="n">
-        <v>0.04804840145753873</v>
+        <v>0.03070853255398958</v>
       </c>
       <c r="D36" t="n">
-        <v>0.04292069312725735</v>
+        <v>0.006845715712852657</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.008829197208972687</v>
+        <v>-0.003981183342925771</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-1.282379224163753</v>
+        <v>-1.936206231204822</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.2221685365681161</v>
+        <v>-0.2445411913953329</v>
       </c>
       <c r="C37" t="n">
-        <v>0.04474148864539645</v>
+        <v>0.02548767314745623</v>
       </c>
       <c r="D37" t="n">
-        <v>0.03955046739072142</v>
+        <v>0.002456841792197529</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.008045181809183025</v>
+        <v>-0.003321506021298277</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>-1.290973972537535</v>
+        <v>-1.914120990588503</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.2172212742248193</v>
+        <v>-0.2334645379349274</v>
       </c>
       <c r="C38" t="n">
-        <v>0.04167421404031228</v>
+        <v>0.02082558523122898</v>
       </c>
       <c r="D38" t="n">
-        <v>0.03636638508913984</v>
+        <v>-0.001466698368816741</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.007334100284288462</v>
+        <v>-0.002748249622872337</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-1.298949226348646</v>
+        <v>-1.892764626914568</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.213090806941925</v>
+        <v>-0.2236218436582191</v>
       </c>
       <c r="C39" t="n">
-        <v>0.03884732531079794</v>
+        <v>0.01667922564586455</v>
       </c>
       <c r="D39" t="n">
-        <v>0.03337966313356831</v>
+        <v>-0.004957523327726419</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.006692836304136179</v>
+        <v>-0.002255011986036276</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-1.30633047333446</v>
+        <v>-1.872121830599931</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.2096923903280952</v>
+        <v>-0.2148779404147087</v>
       </c>
       <c r="C40" t="n">
-        <v>0.03625803467108815</v>
+        <v>0.01300698069802322</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0305967713764025</v>
+        <v>-0.008047804180073876</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.006117780285696717</v>
+        <v>-0.001835421797695067</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>-1.313144548002827</v>
+        <v>-1.852177609392017</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.2069462177960533</v>
+        <v>-0.2071102854145721</v>
       </c>
       <c r="C41" t="n">
-        <v>0.03390071901464566</v>
+        <v>0.009768932387775904</v>
       </c>
       <c r="D41" t="n">
-        <v>0.02802020738255493</v>
+        <v>-0.01076893393933568</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.005605000661558501</v>
+        <v>-0.001483226655444758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>